<commit_message>
update january 2017 onshore oil
</commit_message>
<xml_diff>
--- a/gatsby-site/src/data-graphql/production_volumes.xlsx
+++ b/gatsby-site/src/data-graphql/production_volumes.xlsx
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F626"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A586" workbookViewId="0">
+      <selection activeCell="F608" sqref="F608"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10558,7 +10558,7 @@
         <v>7</v>
       </c>
       <c r="D602" s="11">
-        <v>49699117.337888002</v>
+        <v>2</v>
       </c>
       <c r="E602" s="11">
         <v>77677453.465225995</v>

</xml_diff>